<commit_message>
add Stage 1 and Stage 2
</commit_message>
<xml_diff>
--- a/ChindyChind/evidence.xlsx
+++ b/ChindyChind/evidence.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="87">
   <si>
     <t>TeamName</t>
   </si>
@@ -76,45 +76,12 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -143,13 +110,208 @@
   </si>
   <si>
     <t>omniflix1fhq5uchpnkw9jagsy6txfn6r83gt5wce64cpym</t>
+  </si>
+  <si>
+    <t>92242336692AFFB7D5388A70BD3BCDBA1D0BBB5477F09CB0E15B7FD30D75B01D</t>
+  </si>
+  <si>
+    <t>littlepigeon</t>
+  </si>
+  <si>
+    <t>91306F227AD93D620FB28393E6578F7EDE807E7FE0F2E6D4754508639C2C366E</t>
+  </si>
+  <si>
+    <t>pigeoniris1</t>
+  </si>
+  <si>
+    <t>F916CB9588F81780B6343A01C4330A0008FB390147EFDC904A3D30EAA364965F</t>
+  </si>
+  <si>
+    <t>pigeoniris2</t>
+  </si>
+  <si>
+    <t>D9C311CC7A3E665CAFC70932D092283C5AF7676239033EEE715A9D5B2461826D</t>
+  </si>
+  <si>
+    <t>stars1cad93mjyzgr44tsmd2avuat6gc2pe28lrsawj2687e7v5t0a9rpsjt24la</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>F2624EC6BE053E974EC92F690DB5CB9D14091DE3D3C241065A45088CFADB7D58</t>
+  </si>
+  <si>
+    <t>ibc/91B315CA4900FDDE205A3E818670DF33ED11D6ED807AA7551C949B08259F6580</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>BB51389D2164DCCA3B18A5B37C20EDA5930AB1C0285705CB1480F01534F11559</t>
+  </si>
+  <si>
+    <t>06447094F400141BE39E973B3E92265F592E70033C5B5CE429AE1292568423C1</t>
+  </si>
+  <si>
+    <t>ibc/16D2981580F3C64330CE6E13344E32B843D65C5A5BAC04B769EDC5E60C0118DC</t>
+  </si>
+  <si>
+    <t>pigeoniris3</t>
+  </si>
+  <si>
+    <t>ibc/93F1135F086B82027306140484350BE40CE18B434299D727BEDD15DD1945000D</t>
+  </si>
+  <si>
+    <t>pigeoniris4</t>
+  </si>
+  <si>
+    <t>ibc/9B3E483D9BC9C3B1116451777607DB1BF67E87E40D43482471B787F013F991FC</t>
+  </si>
+  <si>
+    <t>pigeoniris5</t>
+  </si>
+  <si>
+    <t>ibc/7D5111E3816ED6B31FE2BE4C9A84BFBB0814CCF478BB6D379C98DA7808E9B7D6</t>
+  </si>
+  <si>
+    <t>pigeoniris6</t>
+  </si>
+  <si>
+    <t>ibc/F3582318AA07E5BFEBC025400E588182EC04F6B506CE7E92E304D750187B7E7A</t>
+  </si>
+  <si>
+    <t>pigeoniris7</t>
+  </si>
+  <si>
+    <t>ibc/8930DD050BD58E6CEDE21253959A8F7CC13E5D143690EAFBB4A8CCC80E42EC8A</t>
+  </si>
+  <si>
+    <t>pigeoniris8</t>
+  </si>
+  <si>
+    <t>9B5DAB1E49D3CEF33389CFC72F39461ED52BE2B094ACA80600661D949C2ECFD7</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>19DF045F3AB788744C7C58D7F7DEB6DB43E74808C3EA65A76AD80EA503C710B4</t>
+  </si>
+  <si>
+    <t>6D2EFA8A21CF1A1AFD72FCB141F8A2A07156059B2716FD4826B008473268B360</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>125887462E3EFC774307A62C93127DE327DA48FD5048AE85F28F7115DF2A015E</t>
+  </si>
+  <si>
+    <t>EC5FE600C3AD9B53D11ED762EAE75205DA9AF33A74F60C44AECE60A5A2DF3504</t>
+  </si>
+  <si>
+    <t>A00B36CF995ED8CE030D87B9FF49DD99447993C9AAE336D1DBAF1993A3B0323B</t>
+  </si>
+  <si>
+    <t>DF4630995F249FDE2B0A8EE28969EA3413FF3E51CD64B3411F01C78597F3FBF1</t>
+  </si>
+  <si>
+    <t>9A52CEA5B04455A1304E0380C4FE06B08D1835E0B5FE71E42AD844277E03EF04</t>
+  </si>
+  <si>
+    <t>0B9B9ADD18DBE20EC14E8D4B66ED79CA291A762657C734BC45FDD534D6F17120</t>
+  </si>
+  <si>
+    <t>67FE6AABE25D08FA6B9B0A47C721E7A7B0FC128F20DE23D7BA763C2AC908B13E</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>786396118EA75BE59DAC05DCF44A689C1D29CFA622AA20A5982E2AE418D8BAFB</t>
+  </si>
+  <si>
+    <t>21A13C27E2C79ADCA4B310268629EB9B26DD078284979B73DE4E4585A4BF1A11</t>
+  </si>
+  <si>
+    <t>A4D917B87518CA3D5BB4CBE34D805A81FBAA1C25EBF4A824C9BC342926AD1CE3</t>
+  </si>
+  <si>
+    <t>08049DACC4148A6BC0EC690EA1C9358476316D5C17995AF7A370CA35C78052DE</t>
+  </si>
+  <si>
+    <t>B7FB5487036ADD4DF670B4C0A61DC691AECB4D0310F25588AC9DF508427CE944</t>
+  </si>
+  <si>
+    <t>DF1D1B65D1ECA1713C7E8A964D76029D42C64746FE8C1B7E94AE6AA486FCB508</t>
+  </si>
+  <si>
+    <t>05B1A749ECED714EB0A1D11FA32B4EB958C1CB42561BAF570E8EDFAD23CB96B3</t>
+  </si>
+  <si>
+    <t>E081F5933D9DB637B8E184D169CE5EB0284541ED5EBADB70AB3D0092DD7183BA</t>
+  </si>
+  <si>
+    <t>6C200E7B83D6C6A86031372F90DD3578F0B61DF9E2DE07AF9B4100B783C883C2</t>
+  </si>
+  <si>
+    <t>A1AF60B83A9D8FA5DD8551D599250AB5B94948D6A9EFAF16A79515E96832FAD7</t>
+  </si>
+  <si>
+    <t>543662ADF918B4B8741F94AE0739FBF40112E2A3FD7DED0289978295A5BE740C</t>
+  </si>
+  <si>
+    <t>318A264E17B5201D83E0B5E9FE6B7249B29E7BCF4C12C2AF93B8C343C896B81D</t>
+  </si>
+  <si>
+    <t>01C79B7AFDD8EBE7E302176B1E546DDE84457397CB9AA4BE60670845397E363E</t>
+  </si>
+  <si>
+    <t>07251625B24DB570FC18B509A159EB09041839856161257D3F6A6DC3858D7474</t>
+  </si>
+  <si>
+    <t>24907587EBB4D0E72624D28151F09C035BC6A4366744965B981E4052EAEFFF4C</t>
+  </si>
+  <si>
+    <t>75B4D72CA9602E2BC5C2642FD9F0221B8B5F97DAB2052EAA47F4E9AF88EF95F6</t>
+  </si>
+  <si>
+    <t>38E0FECF1E01E982C24512B2448F1DF8626584FC69217DB62444B8E891A906F2</t>
+  </si>
+  <si>
+    <t>B38D9A34C51A35ACEB65BB9B9E79EFD2C32FF06DE249D09C456B5C4ECAEC0827</t>
+  </si>
+  <si>
+    <t>92932704B9E154FE79DCFCD6809DB7F2FF0A61811F78B7A710C70559A68D47B9</t>
+  </si>
+  <si>
+    <t>646991FF5B8BA87EAB7FA60C928B4603B4EA21DFEFC3A150E29056A456902870</t>
+  </si>
+  <si>
+    <t>2685C83D51F9AA2B90F45D4470876EF4C85ABDB3FAB88ADD0331F0ACB056F48C</t>
+  </si>
+  <si>
+    <t>4C3ADB8BB15DEE36BFB5B7B62B24EE8BE7CE73DE21AB6DC3B32FCFAD6520A2B2</t>
+  </si>
+  <si>
+    <t>E14F684DD3BA051DEB7D97D643B4C2F347973EC302129A622FF45DA2B9B21D4F</t>
+  </si>
+  <si>
+    <t>BA6E617EB27F972F928E6ADC6BC08EE79195ECA89F9166F4F766B14D4CB23389</t>
+  </si>
+  <si>
+    <t>4943E0FDE0A39A6DFAF380E3D162692BDEE010BE8696518936A1E45D9924769D</t>
+  </si>
+  <si>
+    <t>696263CE4AEEA049D04BD510B2A005044C0293346A925EE13A7B1C3F6C990306</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,6 +323,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -210,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -225,6 +394,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -571,7 +744,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,28 +787,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +821,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -661,15 +836,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -695,15 +872,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +893,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -729,15 +908,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -763,15 +944,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -782,14 +963,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -797,43 +980,470 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -841,322 +1451,55 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
+      <c r="A4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1183,12 +1526,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1215,12 +1558,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1247,12 +1590,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1281,12 +1624,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1312,12 +1655,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1327,9 +1670,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1345,18 +1690,29 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +1725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1386,24 +1744,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1416,7 +1774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1433,24 +1793,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1480,24 +1842,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1528,24 +1892,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1571,15 +1937,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1592,7 +1958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1605,15 +1973,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>